<commit_message>
8 Equipment tables DONE
</commit_message>
<xml_diff>
--- a/JEM schema change log.xlsx
+++ b/JEM schema change log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjamads\Desktop\JEM Schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjamads\Desktop\git-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017953BE-2B9A-4883-93E0-5949ED9652AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636AAF9B-662C-4458-AE6E-B15DE55F8B6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>table name</t>
   </si>
@@ -114,14 +114,86 @@
     <t>git branch name</t>
   </si>
   <si>
-    <t>26Dec_Equipment</t>
+    <t>EquipmentTemplate</t>
+  </si>
+  <si>
+    <t>TemplateName</t>
+  </si>
+  <si>
+    <t>TemplateShortName</t>
+  </si>
+  <si>
+    <t>UnitType</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>EquipmentTypeTemplateMapping</t>
+  </si>
+  <si>
+    <t>EquipmentTemplatePointMapping</t>
+  </si>
+  <si>
+    <t>EquipmentPlantRoomTemplateMapping</t>
+  </si>
+  <si>
+    <t>EquipmentFaultTimeMachineDetails</t>
+  </si>
+  <si>
+    <t>PointID</t>
+  </si>
+  <si>
+    <t>hasPoint</t>
+  </si>
+  <si>
+    <t>DataSourceID</t>
+  </si>
+  <si>
+    <t>hasDataSource</t>
+  </si>
+  <si>
+    <t>EquipmentID</t>
+  </si>
+  <si>
+    <t>hasEquipment</t>
+  </si>
+  <si>
+    <t>FilterBy</t>
+  </si>
+  <si>
+    <t>FilterBy( attribute of relation "hasEquipmentType" )</t>
+  </si>
+  <si>
+    <t>PlantRoomTemplate</t>
+  </si>
+  <si>
+    <t>hasPlantRoomTemplate</t>
+  </si>
+  <si>
+    <t>IsProcessed</t>
+  </si>
+  <si>
+    <t>RowKey</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>hasRule</t>
+  </si>
+  <si>
+    <t>RuleID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,12 +320,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -457,7 +523,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -587,43 +653,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -661,7 +690,7 @@
     <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -669,39 +698,32 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1025,44 +1047,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="34.21875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="34.21875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1070,37 +1091,37 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>43460</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>29</v>
+      <c r="C2" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1108,33 +1129,33 @@
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1142,113 +1163,408 @@
       <c r="A6" s="8">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10">
+        <v>43461</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>5</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>6</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>7</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>8</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="18">
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="C13:C29"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B13:B29"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D24:D29"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>

</xml_diff>

<commit_message>
Energy 5 tables completed
</commit_message>
<xml_diff>
--- a/JEM schema change log.xlsx
+++ b/JEM schema change log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjamads\Desktop\git-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755552A2-43A0-4C10-BCBD-B949EEB82997}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5CDD8F-8244-40DE-AEB5-C3E0CBA5D935}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="153">
   <si>
     <t>table name</t>
   </si>
@@ -322,13 +322,175 @@
   </si>
   <si>
     <t>hasEquipmentTemplate</t>
+  </si>
+  <si>
+    <t>EnergyImpact</t>
+  </si>
+  <si>
+    <t>hasBuilding</t>
+  </si>
+  <si>
+    <t>UnitID</t>
+  </si>
+  <si>
+    <t>hasUnit</t>
+  </si>
+  <si>
+    <t>hasEnergyImpactType</t>
+  </si>
+  <si>
+    <t>EnergyImpactTypeID</t>
+  </si>
+  <si>
+    <t>FuelConsumptionUnitPrice</t>
+  </si>
+  <si>
+    <t>ElectricalConsumptionUnitPrice</t>
+  </si>
+  <si>
+    <t>CreatedBy</t>
+  </si>
+  <si>
+    <t>UpdatedBy</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>UpdatedDate</t>
+  </si>
+  <si>
+    <t>EnergyImpactMonthlyConsumption</t>
+  </si>
+  <si>
+    <t>CommodityID</t>
+  </si>
+  <si>
+    <t>hasCommodity</t>
+  </si>
+  <si>
+    <t>EnergyImpactID</t>
+  </si>
+  <si>
+    <t>hasEnergyImpact</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>MonthlyConumptionValuePerHour</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EnergyImpactOATConsumption</t>
+  </si>
+  <si>
+    <t>MinOATRangeStartValue</t>
+  </si>
+  <si>
+    <t>MinOATRangeEndValue</t>
+  </si>
+  <si>
+    <t>MinConsumptionValuePerHour</t>
+  </si>
+  <si>
+    <t>MaxOatRangeStartValue</t>
+  </si>
+  <si>
+    <t>MaxOatRangeEndValue</t>
+  </si>
+  <si>
+    <t>MaxConsumptionValuePerHour</t>
+  </si>
+  <si>
+    <t>EnergyImpactScalingFactor</t>
+  </si>
+  <si>
+    <t>ApplyToImpact</t>
+  </si>
+  <si>
+    <t>ScalingVariableLogic</t>
+  </si>
+  <si>
+    <t>ScalingVariableRangeFrom</t>
+  </si>
+  <si>
+    <t>ScalingVariableRangeTo</t>
+  </si>
+  <si>
+    <t>ImpactScalingFactorFrom</t>
+  </si>
+  <si>
+    <t>ImpactScalingFactorTo</t>
+  </si>
+  <si>
+    <t>EnergyImpactCalcDetails</t>
+  </si>
+  <si>
+    <t>FaultAssetMappingId</t>
+  </si>
+  <si>
+    <t>IsFault</t>
+  </si>
+  <si>
+    <t>OccuranceTime</t>
+  </si>
+  <si>
+    <t>ToTimestamp</t>
+  </si>
+  <si>
+    <t>insertionTimestamp</t>
+  </si>
+  <si>
+    <t>AvgOATCalculate</t>
+  </si>
+  <si>
+    <t>ConsumptionPerHour</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>ScalingApplicable</t>
+  </si>
+  <si>
+    <t>PointAValue</t>
+  </si>
+  <si>
+    <t>PointBValue</t>
+  </si>
+  <si>
+    <t>ScalingVariablelogiccalculationvalue</t>
+  </si>
+  <si>
+    <t>ScalingVariable</t>
+  </si>
+  <si>
+    <t>ScalingFactorCalcFormula</t>
+  </si>
+  <si>
+    <t>3JAN_Energy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,6 +637,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -870,7 +1037,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -895,19 +1062,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -918,6 +1079,18 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1240,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,16 +1454,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="17">
         <v>43460</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1304,10 +1477,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1319,12 +1492,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1338,10 +1511,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1353,12 +1526,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1372,10 +1545,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1387,10 +1560,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1402,10 +1575,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1417,10 +1590,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1432,10 +1605,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1447,10 +1620,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1462,16 +1635,16 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="16">
         <v>4</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="17">
         <v>43461</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1485,10 +1658,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1500,10 +1673,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1515,10 +1688,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
@@ -1530,10 +1703,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1545,12 +1718,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="16">
         <v>5</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1564,10 +1737,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="6" t="s">
         <v>44</v>
       </c>
@@ -1579,12 +1752,12 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="16">
         <v>6</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1598,10 +1771,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="3" t="s">
         <v>40</v>
       </c>
@@ -1613,10 +1786,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="6" t="s">
         <v>42</v>
       </c>
@@ -1631,8 +1804,8 @@
       <c r="A23" s="7">
         <v>7</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="7" t="s">
         <v>36</v>
       </c>
@@ -1647,12 +1820,12 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="16">
         <v>8</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E24" s="6" t="s">
@@ -1666,10 +1839,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="6" t="s">
         <v>49</v>
       </c>
@@ -1681,10 +1854,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="6" t="s">
         <v>50</v>
       </c>
@@ -1696,10 +1869,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
       <c r="E27" s="6" t="s">
         <v>51</v>
       </c>
@@ -1711,10 +1884,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="6" t="s">
         <v>53</v>
       </c>
@@ -1726,10 +1899,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
       <c r="E29" s="6" t="s">
         <v>42</v>
       </c>
@@ -1744,10 +1917,10 @@
       <c r="A30" s="7">
         <v>9</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="13">
         <v>43467</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="8" t="s">
@@ -1764,12 +1937,12 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="A31" s="10">
         <v>10</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="12" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E31" s="6" t="s">
@@ -1783,10 +1956,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="6" t="s">
         <v>61</v>
       </c>
@@ -1801,8 +1974,8 @@
       <c r="A33" s="5">
         <v>11</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="5" t="s">
         <v>63</v>
       </c>
@@ -1817,12 +1990,12 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
-        <v>12</v>
-      </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="12" t="s">
+      <c r="A34" s="10">
+        <v>12</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="10" t="s">
         <v>64</v>
       </c>
       <c r="E34" s="6" t="s">
@@ -1836,10 +2009,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="6" t="s">
         <v>66</v>
       </c>
@@ -1851,10 +2024,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="6" t="s">
         <v>67</v>
       </c>
@@ -1866,10 +2039,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="6" t="s">
         <v>71</v>
       </c>
@@ -1881,10 +2054,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="6" t="s">
         <v>68</v>
       </c>
@@ -1896,10 +2069,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
       <c r="E39" s="6" t="s">
         <v>42</v>
       </c>
@@ -1914,8 +2087,8 @@
       <c r="A40" s="5">
         <v>13</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="8" t="s">
         <v>72</v>
       </c>
@@ -1930,12 +2103,12 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
+      <c r="A41" s="10">
         <v>14</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="12" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="10" t="s">
         <v>74</v>
       </c>
       <c r="E41" s="6" t="s">
@@ -1949,10 +2122,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
       <c r="E42" s="6" t="s">
         <v>77</v>
       </c>
@@ -1964,10 +2137,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="13"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="12"/>
       <c r="E43" s="6" t="s">
         <v>78</v>
       </c>
@@ -1979,12 +2152,12 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
+      <c r="A44" s="10">
         <v>15</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="12" t="s">
+      <c r="B44" s="14"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="10" t="s">
         <v>79</v>
       </c>
       <c r="E44" s="6" t="s">
@@ -1998,10 +2171,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
       <c r="E45" s="6" t="s">
         <v>81</v>
       </c>
@@ -2013,10 +2186,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="13"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="12"/>
       <c r="E46" s="6" t="s">
         <v>82</v>
       </c>
@@ -2031,8 +2204,8 @@
       <c r="A47" s="5">
         <v>16</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="5" t="s">
         <v>86</v>
       </c>
@@ -2047,12 +2220,12 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="12">
+      <c r="A48" s="10">
         <v>17</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="12" t="s">
+      <c r="B48" s="14"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="10" t="s">
         <v>88</v>
       </c>
       <c r="E48" s="6" t="s">
@@ -2066,10 +2239,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="13"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="6" t="s">
         <v>89</v>
       </c>
@@ -2081,12 +2254,12 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="12">
+      <c r="A50" s="10">
         <v>18</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="12" t="s">
+      <c r="B50" s="14"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E50" s="6" t="s">
@@ -2100,10 +2273,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
       <c r="E51" s="6" t="s">
         <v>93</v>
       </c>
@@ -2115,10 +2288,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
       <c r="E52" s="6" t="s">
         <v>94</v>
       </c>
@@ -2130,10 +2303,10 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
       <c r="E53" s="6" t="s">
         <v>95</v>
       </c>
@@ -2144,8 +2317,1235 @@
         <v>13</v>
       </c>
     </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
+        <v>19</v>
+      </c>
+      <c r="B54" s="13">
+        <v>43468</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="10">
+        <v>20</v>
+      </c>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="11"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="11"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="11"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="12"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
+        <v>21</v>
+      </c>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F87" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F88" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="11"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F89" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F90" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F91" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F92" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="11"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F93" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="12"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F95" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="10">
+        <v>22</v>
+      </c>
+      <c r="B96" s="11"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="11"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="11"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="11"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="11"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
+      <c r="E102" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="11"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="11"/>
+      <c r="B104" s="11"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F104" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F105" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F106" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="11"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F107" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="12"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F108" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="10">
+        <v>23</v>
+      </c>
+      <c r="B109" s="11"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="11"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="11"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="11"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="11"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="11"/>
+      <c r="B115" s="11"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="11"/>
+      <c r="B116" s="11"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="11"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="11"/>
+      <c r="B118" s="11"/>
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="11"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="11"/>
+      <c r="B122" s="11"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F122" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="11"/>
+      <c r="B123" s="11"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="11"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
+      <c r="E124" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="11"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
+      <c r="E125" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F125" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="11"/>
+      <c r="B126" s="11"/>
+      <c r="C126" s="11"/>
+      <c r="D126" s="11"/>
+      <c r="E126" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F126" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="11"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F127" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="11"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="11"/>
+      <c r="D128" s="11"/>
+      <c r="E128" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F128" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="12"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F129" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E130" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E131" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E132" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="44">
+    <mergeCell ref="D96:D108"/>
+    <mergeCell ref="A96:A108"/>
+    <mergeCell ref="D109:D129"/>
+    <mergeCell ref="A109:A129"/>
+    <mergeCell ref="C54:C129"/>
+    <mergeCell ref="B54:B129"/>
+    <mergeCell ref="D54:D66"/>
+    <mergeCell ref="A54:A66"/>
+    <mergeCell ref="D67:D81"/>
+    <mergeCell ref="D82:D95"/>
+    <mergeCell ref="A67:A81"/>
+    <mergeCell ref="A82:A95"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="C13:C29"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B13:B29"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C2:C12"/>
     <mergeCell ref="D50:D53"/>
     <mergeCell ref="B30:B53"/>
     <mergeCell ref="C30:C53"/>
@@ -2160,24 +3560,6 @@
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="D34:D39"/>
     <mergeCell ref="D41:D43"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="D6:D12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C12"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="C13:C29"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B13:B29"/>
-    <mergeCell ref="A24:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
after hour tables done
</commit_message>
<xml_diff>
--- a/JEM schema change log.xlsx
+++ b/JEM schema change log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjamads\Desktop\git-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391EEEE8-7F91-4A32-BBDE-6741DA2BE3A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7479B267-098D-474B-9028-CA5877011143}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="222">
   <si>
     <t>table name</t>
   </si>
@@ -568,6 +568,129 @@
   </si>
   <si>
     <t>isMeter( attribute of relation "hasSystem" )</t>
+  </si>
+  <si>
+    <t>AfterHourZone</t>
+  </si>
+  <si>
+    <t>CreatedOn</t>
+  </si>
+  <si>
+    <t>hasSpace</t>
+  </si>
+  <si>
+    <t>hasTenant</t>
+  </si>
+  <si>
+    <t>TenantID</t>
+  </si>
+  <si>
+    <t>createdBy</t>
+  </si>
+  <si>
+    <t>AfterHourZoneName</t>
+  </si>
+  <si>
+    <t>AfterHourSwitchRate</t>
+  </si>
+  <si>
+    <t>EffectiveDate</t>
+  </si>
+  <si>
+    <t>AppliedRate</t>
+  </si>
+  <si>
+    <t>AfterHourZoneID</t>
+  </si>
+  <si>
+    <t>hasAfterHourZone</t>
+  </si>
+  <si>
+    <t>AfterHourCommandType</t>
+  </si>
+  <si>
+    <t>CommandType</t>
+  </si>
+  <si>
+    <t>AfterHourCommandStatus</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>AfterHourCommand</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>RequestedBy</t>
+  </si>
+  <si>
+    <t>RequestedOn</t>
+  </si>
+  <si>
+    <t>StatusID</t>
+  </si>
+  <si>
+    <t>CommandTypeID</t>
+  </si>
+  <si>
+    <t>hasStatus</t>
+  </si>
+  <si>
+    <t>requestedBy</t>
+  </si>
+  <si>
+    <t>hasAfterHourCommandType</t>
+  </si>
+  <si>
+    <t>AfterHourZonePointMapping</t>
+  </si>
+  <si>
+    <t>CommandPointID</t>
+  </si>
+  <si>
+    <t>StatusPointID</t>
+  </si>
+  <si>
+    <t>hasCommandPoint</t>
+  </si>
+  <si>
+    <t>hasStatusPoint</t>
+  </si>
+  <si>
+    <t>hasUser</t>
+  </si>
+  <si>
+    <t>AfterHourZoneUserMapping</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>AfterHourCommandDetails</t>
+  </si>
+  <si>
+    <t>CommandID</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>ActualStartTime</t>
+  </si>
+  <si>
+    <t>ActualEndTime</t>
+  </si>
+  <si>
+    <t>hasAfterHourCommand</t>
+  </si>
+  <si>
+    <t>AfterHourCommandAudit</t>
+  </si>
+  <si>
+    <t>4JAN_AfterHourTables</t>
   </si>
 </sst>
 </file>
@@ -1152,25 +1275,25 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1494,17 +1617,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="5"/>
     <col min="2" max="2" width="13.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="34.21875" style="6" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
@@ -1535,16 +1658,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="18">
         <v>43460</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1558,10 +1681,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1573,12 +1696,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="17">
         <v>2</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1592,10 +1715,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1607,12 +1730,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="17">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="15" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="17" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1626,10 +1749,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="15"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1641,10 +1764,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="15"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1656,10 +1779,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1671,10 +1794,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1686,10 +1809,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1701,10 +1824,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1716,16 +1839,16 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="17">
         <v>4</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="18">
         <v>43461</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="17" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1739,10 +1862,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1754,10 +1877,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1769,10 +1892,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
@@ -1784,10 +1907,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1799,12 +1922,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="A18" s="17">
         <v>5</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1818,10 +1941,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="6" t="s">
         <v>44</v>
       </c>
@@ -1833,12 +1956,12 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="A20" s="17">
         <v>6</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1852,10 +1975,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="3" t="s">
         <v>40</v>
       </c>
@@ -1867,10 +1990,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="6" t="s">
         <v>42</v>
       </c>
@@ -1885,8 +2008,8 @@
       <c r="A23" s="8">
         <v>7</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="8" t="s">
         <v>36</v>
       </c>
@@ -1901,12 +2024,12 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="17">
         <v>8</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E24" s="6" t="s">
@@ -1920,10 +2043,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
       <c r="E25" s="6" t="s">
         <v>49</v>
       </c>
@@ -1935,10 +2058,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="6" t="s">
         <v>50</v>
       </c>
@@ -1950,10 +2073,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
       <c r="E27" s="6" t="s">
         <v>51</v>
       </c>
@@ -1965,10 +2088,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="6" t="s">
         <v>53</v>
       </c>
@@ -1980,10 +2103,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="6" t="s">
         <v>42</v>
       </c>
@@ -2021,8 +2144,8 @@
       <c r="A31" s="11">
         <v>10</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="11" t="s">
         <v>58</v>
       </c>
@@ -2037,10 +2160,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="6" t="s">
         <v>61</v>
       </c>
@@ -2055,8 +2178,8 @@
       <c r="A33" s="8">
         <v>11</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="12"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="8" t="s">
         <v>63</v>
       </c>
@@ -2074,8 +2197,8 @@
       <c r="A34" s="11">
         <v>12</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="12"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="11" t="s">
         <v>64</v>
       </c>
@@ -2090,10 +2213,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="6" t="s">
         <v>66</v>
       </c>
@@ -2105,10 +2228,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="6" t="s">
         <v>67</v>
       </c>
@@ -2120,10 +2243,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
       <c r="E37" s="6" t="s">
         <v>71</v>
       </c>
@@ -2135,10 +2258,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
       <c r="E38" s="6" t="s">
         <v>68</v>
       </c>
@@ -2150,10 +2273,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="12"/>
       <c r="E39" s="6" t="s">
         <v>42</v>
       </c>
@@ -2168,8 +2291,8 @@
       <c r="A40" s="8">
         <v>13</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="12"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="8" t="s">
         <v>72</v>
       </c>
@@ -2187,8 +2310,8 @@
       <c r="A41" s="11">
         <v>14</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="12"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="11" t="s">
         <v>74</v>
       </c>
@@ -2203,10 +2326,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
       <c r="E42" s="6" t="s">
         <v>77</v>
       </c>
@@ -2218,10 +2341,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="12"/>
       <c r="E43" s="6" t="s">
         <v>78</v>
       </c>
@@ -2236,8 +2359,8 @@
       <c r="A44" s="11">
         <v>15</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="12"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="11" t="s">
         <v>79</v>
       </c>
@@ -2252,10 +2375,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
       <c r="E45" s="6" t="s">
         <v>81</v>
       </c>
@@ -2267,10 +2390,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="13"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="12"/>
       <c r="E46" s="6" t="s">
         <v>82</v>
       </c>
@@ -2285,8 +2408,8 @@
       <c r="A47" s="8">
         <v>16</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="12"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="8" t="s">
         <v>86</v>
       </c>
@@ -2304,8 +2427,8 @@
       <c r="A48" s="11">
         <v>17</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="12"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="11" t="s">
         <v>88</v>
       </c>
@@ -2320,10 +2443,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="6" t="s">
         <v>89</v>
       </c>
@@ -2338,8 +2461,8 @@
       <c r="A50" s="11">
         <v>18</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="12"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="13"/>
       <c r="D50" s="11" t="s">
         <v>90</v>
       </c>
@@ -2354,10 +2477,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
       <c r="E51" s="6" t="s">
         <v>93</v>
       </c>
@@ -2369,10 +2492,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="6" t="s">
         <v>94</v>
       </c>
@@ -2384,10 +2507,10 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
       <c r="E53" s="6" t="s">
         <v>95</v>
       </c>
@@ -2422,10 +2545,10 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
       <c r="E55" s="6" t="s">
         <v>17</v>
       </c>
@@ -2437,10 +2560,10 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="6" t="s">
         <v>42</v>
       </c>
@@ -2452,10 +2575,10 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
       <c r="E57" s="6" t="s">
         <v>53</v>
       </c>
@@ -2467,10 +2590,10 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
       <c r="E58" s="6" t="s">
         <v>101</v>
       </c>
@@ -2482,10 +2605,10 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
       <c r="E59" s="6" t="s">
         <v>104</v>
       </c>
@@ -2497,10 +2620,10 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
       <c r="E60" s="6" t="s">
         <v>105</v>
       </c>
@@ -2512,10 +2635,10 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
+      <c r="A61" s="13"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
       <c r="E61" s="6" t="s">
         <v>106</v>
       </c>
@@ -2527,10 +2650,10 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
       <c r="E62" s="6" t="s">
         <v>107</v>
       </c>
@@ -2542,10 +2665,10 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
       <c r="E63" s="10" t="s">
         <v>108</v>
       </c>
@@ -2557,10 +2680,10 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
       <c r="E64" s="10" t="s">
         <v>109</v>
       </c>
@@ -2572,10 +2695,10 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
       <c r="E65" s="10" t="s">
         <v>110</v>
       </c>
@@ -2587,10 +2710,10 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
+      <c r="A66" s="12"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="12"/>
       <c r="E66" s="10" t="s">
         <v>111</v>
       </c>
@@ -2605,8 +2728,8 @@
       <c r="A67" s="11">
         <v>20</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="12"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="13"/>
       <c r="D67" s="11" t="s">
         <v>112</v>
       </c>
@@ -2621,10 +2744,10 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
       <c r="E68" s="6" t="s">
         <v>101</v>
       </c>
@@ -2636,10 +2759,10 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
       <c r="E69" s="6" t="s">
         <v>115</v>
       </c>
@@ -2651,10 +2774,10 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
       <c r="E70" s="10" t="s">
         <v>117</v>
       </c>
@@ -2666,10 +2789,10 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
       <c r="E71" s="10" t="s">
         <v>118</v>
       </c>
@@ -2681,10 +2804,10 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
       <c r="E72" s="10" t="s">
         <v>119</v>
       </c>
@@ -2696,10 +2819,10 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
       <c r="E73" s="10" t="s">
         <v>120</v>
       </c>
@@ -2711,10 +2834,10 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
       <c r="E74" s="10" t="s">
         <v>121</v>
       </c>
@@ -2726,10 +2849,10 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
+      <c r="A75" s="13"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
       <c r="E75" s="10" t="s">
         <v>122</v>
       </c>
@@ -2741,10 +2864,10 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="12"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
       <c r="E76" s="10" t="s">
         <v>51</v>
       </c>
@@ -2756,10 +2879,10 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="12"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
+      <c r="A77" s="13"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
       <c r="E77" s="10" t="s">
         <v>107</v>
       </c>
@@ -2771,10 +2894,10 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
+      <c r="A78" s="13"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
       <c r="E78" s="10" t="s">
         <v>108</v>
       </c>
@@ -2786,10 +2909,10 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
+      <c r="A79" s="13"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
       <c r="E79" s="10" t="s">
         <v>109</v>
       </c>
@@ -2801,10 +2924,10 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
+      <c r="A80" s="13"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
       <c r="E80" s="10" t="s">
         <v>110</v>
       </c>
@@ -2816,10 +2939,10 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="13"/>
+      <c r="A81" s="12"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="12"/>
       <c r="E81" s="10" t="s">
         <v>111</v>
       </c>
@@ -2834,8 +2957,8 @@
       <c r="A82" s="11">
         <v>21</v>
       </c>
-      <c r="B82" s="17"/>
-      <c r="C82" s="12"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="13"/>
       <c r="D82" s="11" t="s">
         <v>123</v>
       </c>
@@ -2850,10 +2973,10 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="12"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
+      <c r="A83" s="13"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
       <c r="E83" s="6" t="s">
         <v>101</v>
       </c>
@@ -2865,10 +2988,10 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="12"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
+      <c r="A84" s="13"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
       <c r="E84" s="6" t="s">
         <v>115</v>
       </c>
@@ -2880,10 +3003,10 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="12"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="A85" s="13"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
       <c r="E85" s="9" t="s">
         <v>124</v>
       </c>
@@ -2895,10 +3018,10 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
+      <c r="A86" s="13"/>
+      <c r="B86" s="15"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
       <c r="E86" s="9" t="s">
         <v>125</v>
       </c>
@@ -2910,10 +3033,10 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
+      <c r="A87" s="13"/>
+      <c r="B87" s="15"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
       <c r="E87" s="9" t="s">
         <v>126</v>
       </c>
@@ -2925,10 +3048,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
+      <c r="A88" s="13"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
       <c r="E88" s="9" t="s">
         <v>127</v>
       </c>
@@ -2940,10 +3063,10 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
+      <c r="A89" s="13"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
       <c r="E89" s="9" t="s">
         <v>128</v>
       </c>
@@ -2955,10 +3078,10 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
+      <c r="A90" s="13"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
       <c r="E90" s="9" t="s">
         <v>129</v>
       </c>
@@ -2970,10 +3093,10 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="12"/>
-      <c r="D91" s="12"/>
+      <c r="A91" s="13"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
       <c r="E91" s="10" t="s">
         <v>107</v>
       </c>
@@ -2985,10 +3108,10 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="12"/>
+      <c r="A92" s="13"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
       <c r="E92" s="10" t="s">
         <v>108</v>
       </c>
@@ -3000,10 +3123,10 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
+      <c r="A93" s="13"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
       <c r="E93" s="10" t="s">
         <v>109</v>
       </c>
@@ -3015,10 +3138,10 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
-      <c r="B94" s="17"/>
-      <c r="C94" s="12"/>
-      <c r="D94" s="12"/>
+      <c r="A94" s="13"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
       <c r="E94" s="10" t="s">
         <v>110</v>
       </c>
@@ -3030,10 +3153,10 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="13"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="13"/>
+      <c r="A95" s="12"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="12"/>
       <c r="E95" s="10" t="s">
         <v>111</v>
       </c>
@@ -3048,8 +3171,8 @@
       <c r="A96" s="11">
         <v>22</v>
       </c>
-      <c r="B96" s="17"/>
-      <c r="C96" s="12"/>
+      <c r="B96" s="15"/>
+      <c r="C96" s="13"/>
       <c r="D96" s="11" t="s">
         <v>130</v>
       </c>
@@ -3064,10 +3187,10 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
+      <c r="A97" s="13"/>
+      <c r="B97" s="15"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
       <c r="E97" s="6" t="s">
         <v>115</v>
       </c>
@@ -3079,10 +3202,10 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
+      <c r="A98" s="13"/>
+      <c r="B98" s="15"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
       <c r="E98" s="6" t="s">
         <v>131</v>
       </c>
@@ -3094,10 +3217,10 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="17"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
+      <c r="A99" s="13"/>
+      <c r="B99" s="15"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
       <c r="E99" s="6" t="s">
         <v>132</v>
       </c>
@@ -3109,10 +3232,10 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
+      <c r="A100" s="13"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
       <c r="E100" s="6" t="s">
         <v>133</v>
       </c>
@@ -3124,10 +3247,10 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
-      <c r="B101" s="17"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="15"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
       <c r="E101" s="6" t="s">
         <v>134</v>
       </c>
@@ -3139,10 +3262,10 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
-      <c r="B102" s="17"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
+      <c r="A102" s="13"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
       <c r="E102" s="6" t="s">
         <v>135</v>
       </c>
@@ -3154,10 +3277,10 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="12"/>
-      <c r="D103" s="12"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
       <c r="E103" s="6" t="s">
         <v>136</v>
       </c>
@@ -3169,10 +3292,10 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
+      <c r="A104" s="13"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
       <c r="E104" s="10" t="s">
         <v>107</v>
       </c>
@@ -3184,10 +3307,10 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="12"/>
-      <c r="B105" s="17"/>
-      <c r="C105" s="12"/>
-      <c r="D105" s="12"/>
+      <c r="A105" s="13"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
       <c r="E105" s="10" t="s">
         <v>108</v>
       </c>
@@ -3199,10 +3322,10 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="12"/>
-      <c r="B106" s="17"/>
-      <c r="C106" s="12"/>
-      <c r="D106" s="12"/>
+      <c r="A106" s="13"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
       <c r="E106" s="10" t="s">
         <v>109</v>
       </c>
@@ -3214,10 +3337,10 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="12"/>
-      <c r="B107" s="17"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
+      <c r="A107" s="13"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
       <c r="E107" s="10" t="s">
         <v>110</v>
       </c>
@@ -3229,10 +3352,10 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="13"/>
-      <c r="B108" s="17"/>
-      <c r="C108" s="12"/>
-      <c r="D108" s="13"/>
+      <c r="A108" s="12"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="12"/>
       <c r="E108" s="10" t="s">
         <v>111</v>
       </c>
@@ -3247,8 +3370,8 @@
       <c r="A109" s="11">
         <v>23</v>
       </c>
-      <c r="B109" s="17"/>
-      <c r="C109" s="12"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="13"/>
       <c r="D109" s="11" t="s">
         <v>137</v>
       </c>
@@ -3263,10 +3386,10 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="12"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="12"/>
-      <c r="D110" s="12"/>
+      <c r="A110" s="13"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
       <c r="E110" s="6" t="s">
         <v>65</v>
       </c>
@@ -3278,10 +3401,10 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="12"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="12"/>
-      <c r="D111" s="12"/>
+      <c r="A111" s="13"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
       <c r="E111" s="6" t="s">
         <v>138</v>
       </c>
@@ -3293,10 +3416,10 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="12"/>
-      <c r="B112" s="17"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
+      <c r="A112" s="13"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
       <c r="E112" s="6" t="s">
         <v>139</v>
       </c>
@@ -3308,10 +3431,10 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="12"/>
-      <c r="B113" s="17"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="15"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
       <c r="E113" s="6" t="s">
         <v>140</v>
       </c>
@@ -3323,10 +3446,10 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
-      <c r="B114" s="17"/>
-      <c r="C114" s="12"/>
-      <c r="D114" s="12"/>
+      <c r="A114" s="13"/>
+      <c r="B114" s="15"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
       <c r="E114" s="6" t="s">
         <v>141</v>
       </c>
@@ -3338,10 +3461,10 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="12"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="12"/>
-      <c r="D115" s="12"/>
+      <c r="A115" s="13"/>
+      <c r="B115" s="15"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
       <c r="E115" s="6" t="s">
         <v>142</v>
       </c>
@@ -3353,10 +3476,10 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="12"/>
-      <c r="B116" s="17"/>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="15"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
       <c r="E116" s="6" t="s">
         <v>143</v>
       </c>
@@ -3368,10 +3491,10 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="12"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="12"/>
-      <c r="D117" s="12"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="15"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
       <c r="E117" s="6" t="s">
         <v>144</v>
       </c>
@@ -3383,10 +3506,10 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="12"/>
-      <c r="B118" s="17"/>
-      <c r="C118" s="12"/>
-      <c r="D118" s="12"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="15"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
       <c r="E118" s="6" t="s">
         <v>145</v>
       </c>
@@ -3398,10 +3521,10 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="12"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="12"/>
-      <c r="D119" s="12"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="15"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
       <c r="E119" s="6" t="s">
         <v>146</v>
       </c>
@@ -3413,10 +3536,10 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="12"/>
-      <c r="D120" s="12"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
       <c r="E120" s="6" t="s">
         <v>147</v>
       </c>
@@ -3428,10 +3551,10 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="12"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
       <c r="E121" s="6" t="s">
         <v>148</v>
       </c>
@@ -3443,10 +3566,10 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="12"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="12"/>
-      <c r="D122" s="12"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
       <c r="E122" s="6" t="s">
         <v>149</v>
       </c>
@@ -3458,10 +3581,10 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="15"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
       <c r="E123" s="6" t="s">
         <v>150</v>
       </c>
@@ -3473,10 +3596,10 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="12"/>
-      <c r="B124" s="17"/>
-      <c r="C124" s="12"/>
-      <c r="D124" s="12"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="15"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
       <c r="E124" s="6" t="s">
         <v>151</v>
       </c>
@@ -3488,10 +3611,10 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="12"/>
-      <c r="B125" s="17"/>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="15"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
       <c r="E125" s="10" t="s">
         <v>107</v>
       </c>
@@ -3503,10 +3626,10 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="12"/>
-      <c r="B126" s="17"/>
-      <c r="C126" s="12"/>
-      <c r="D126" s="12"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
       <c r="E126" s="10" t="s">
         <v>108</v>
       </c>
@@ -3518,10 +3641,10 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="12"/>
-      <c r="B127" s="17"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="15"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
       <c r="E127" s="10" t="s">
         <v>109</v>
       </c>
@@ -3533,10 +3656,10 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="12"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="12"/>
-      <c r="D128" s="12"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="15"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
       <c r="E128" s="10" t="s">
         <v>110</v>
       </c>
@@ -3548,10 +3671,10 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="12"/>
-      <c r="B129" s="17"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="15"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
       <c r="E129" s="10" t="s">
         <v>111</v>
       </c>
@@ -3563,10 +3686,10 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="12"/>
-      <c r="B130" s="17"/>
-      <c r="C130" s="12"/>
-      <c r="D130" s="12"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="15"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
       <c r="E130" s="6" t="s">
         <v>113</v>
       </c>
@@ -3578,10 +3701,10 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="12"/>
-      <c r="B131" s="17"/>
-      <c r="C131" s="12"/>
-      <c r="D131" s="12"/>
+      <c r="A131" s="13"/>
+      <c r="B131" s="15"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
       <c r="E131" s="6" t="s">
         <v>115</v>
       </c>
@@ -3593,10 +3716,10 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="13"/>
-      <c r="B132" s="18"/>
-      <c r="C132" s="13"/>
-      <c r="D132" s="13"/>
+      <c r="A132" s="12"/>
+      <c r="B132" s="16"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="12"/>
       <c r="E132" s="6" t="s">
         <v>42</v>
       </c>
@@ -3611,8 +3734,12 @@
       <c r="A133" s="8">
         <v>24</v>
       </c>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
+      <c r="B133" s="14">
+        <v>43469</v>
+      </c>
+      <c r="C133" s="11" t="s">
+        <v>221</v>
+      </c>
       <c r="D133" s="8" t="s">
         <v>154</v>
       </c>
@@ -3630,8 +3757,8 @@
       <c r="A134" s="11">
         <v>25</v>
       </c>
-      <c r="B134" s="12"/>
-      <c r="C134" s="12"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
       <c r="D134" s="11" t="s">
         <v>153</v>
       </c>
@@ -3646,10 +3773,10 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="13"/>
-      <c r="B135" s="12"/>
-      <c r="C135" s="12"/>
-      <c r="D135" s="13"/>
+      <c r="A135" s="12"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="12"/>
       <c r="E135" s="6" t="s">
         <v>158</v>
       </c>
@@ -3664,8 +3791,8 @@
       <c r="A136" s="8">
         <v>26</v>
       </c>
-      <c r="B136" s="12"/>
-      <c r="C136" s="12"/>
+      <c r="B136" s="13"/>
+      <c r="C136" s="13"/>
       <c r="D136" s="8" t="s">
         <v>159</v>
       </c>
@@ -3683,8 +3810,8 @@
       <c r="A137" s="11">
         <v>27</v>
       </c>
-      <c r="B137" s="12"/>
-      <c r="C137" s="12"/>
+      <c r="B137" s="13"/>
+      <c r="C137" s="13"/>
       <c r="D137" s="11" t="s">
         <v>161</v>
       </c>
@@ -3699,10 +3826,10 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="12"/>
-      <c r="B138" s="12"/>
-      <c r="C138" s="12"/>
-      <c r="D138" s="12"/>
+      <c r="A138" s="13"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
       <c r="E138" s="3" t="s">
         <v>163</v>
       </c>
@@ -3714,10 +3841,10 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="12"/>
-      <c r="B139" s="12"/>
-      <c r="C139" s="12"/>
-      <c r="D139" s="12"/>
+      <c r="A139" s="13"/>
+      <c r="B139" s="13"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="13"/>
       <c r="E139" s="3" t="s">
         <v>158</v>
       </c>
@@ -3729,10 +3856,10 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="12"/>
-      <c r="B140" s="12"/>
-      <c r="C140" s="12"/>
-      <c r="D140" s="12"/>
+      <c r="A140" s="13"/>
+      <c r="B140" s="13"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
       <c r="E140" s="3" t="s">
         <v>164</v>
       </c>
@@ -3744,10 +3871,10 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="12"/>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
+      <c r="A141" s="13"/>
+      <c r="B141" s="13"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
       <c r="E141" s="3" t="s">
         <v>165</v>
       </c>
@@ -3759,10 +3886,10 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="12"/>
-      <c r="B142" s="12"/>
-      <c r="C142" s="12"/>
-      <c r="D142" s="12"/>
+      <c r="A142" s="13"/>
+      <c r="B142" s="13"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
       <c r="E142" s="3" t="s">
         <v>166</v>
       </c>
@@ -3774,10 +3901,10 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="12"/>
-      <c r="B143" s="12"/>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
       <c r="E143" s="3" t="s">
         <v>167</v>
       </c>
@@ -3789,10 +3916,10 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="12"/>
-      <c r="B144" s="12"/>
-      <c r="C144" s="12"/>
-      <c r="D144" s="12"/>
+      <c r="A144" s="13"/>
+      <c r="B144" s="13"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="13"/>
       <c r="E144" s="3" t="s">
         <v>168</v>
       </c>
@@ -3804,10 +3931,10 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="12"/>
-      <c r="B145" s="12"/>
-      <c r="C145" s="12"/>
-      <c r="D145" s="12"/>
+      <c r="A145" s="13"/>
+      <c r="B145" s="13"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
       <c r="E145" s="3" t="s">
         <v>53</v>
       </c>
@@ -3819,10 +3946,10 @@
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="13"/>
-      <c r="B146" s="12"/>
-      <c r="C146" s="12"/>
-      <c r="D146" s="13"/>
+      <c r="A146" s="12"/>
+      <c r="B146" s="13"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="12"/>
       <c r="E146" s="3" t="s">
         <v>169</v>
       </c>
@@ -3837,8 +3964,8 @@
       <c r="A147" s="8">
         <v>28</v>
       </c>
-      <c r="B147" s="12"/>
-      <c r="C147" s="12"/>
+      <c r="B147" s="13"/>
+      <c r="C147" s="13"/>
       <c r="D147" s="8" t="s">
         <v>172</v>
       </c>
@@ -3856,8 +3983,8 @@
       <c r="A148" s="8">
         <v>29</v>
       </c>
-      <c r="B148" s="12"/>
-      <c r="C148" s="12"/>
+      <c r="B148" s="13"/>
+      <c r="C148" s="13"/>
       <c r="D148" s="8" t="s">
         <v>175</v>
       </c>
@@ -3875,8 +4002,8 @@
       <c r="A149" s="11">
         <v>30</v>
       </c>
-      <c r="B149" s="12"/>
-      <c r="C149" s="12"/>
+      <c r="B149" s="13"/>
+      <c r="C149" s="13"/>
       <c r="D149" s="11" t="s">
         <v>178</v>
       </c>
@@ -3891,10 +4018,10 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="13"/>
+      <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="13"/>
-      <c r="D150" s="13"/>
+      <c r="D150" s="12"/>
       <c r="E150" s="6" t="s">
         <v>179</v>
       </c>
@@ -3905,16 +4032,538 @@
         <v>12</v>
       </c>
     </row>
+    <row r="151" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="11">
+        <v>31</v>
+      </c>
+      <c r="B151" s="13"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="13"/>
+      <c r="B152" s="13"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="13"/>
+      <c r="B153" s="13"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="13"/>
+      <c r="B154" s="13"/>
+      <c r="C154" s="13"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F154" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="12"/>
+      <c r="B155" s="13"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="12"/>
+      <c r="E155" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="11">
+        <v>32</v>
+      </c>
+      <c r="B156" s="13"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="13"/>
+      <c r="B157" s="13"/>
+      <c r="C157" s="13"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F157" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="12"/>
+      <c r="B158" s="13"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="12"/>
+      <c r="E158" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="5">
+        <v>33</v>
+      </c>
+      <c r="B159" s="13"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="5">
+        <v>34</v>
+      </c>
+      <c r="B160" s="13"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F160" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="11">
+        <v>35</v>
+      </c>
+      <c r="B161" s="13"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F161" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G161" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="13"/>
+      <c r="B162" s="13"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F162" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="13"/>
+      <c r="B163" s="13"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="13"/>
+      <c r="B164" s="13"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="13"/>
+      <c r="B165" s="13"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F165" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="13"/>
+      <c r="B166" s="13"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F166" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="13"/>
+      <c r="B167" s="13"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F167" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="12"/>
+      <c r="B168" s="13"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F168" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="11">
+        <v>36</v>
+      </c>
+      <c r="B169" s="13"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F169" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="12"/>
+      <c r="B170" s="13"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F170" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="5">
+        <v>37</v>
+      </c>
+      <c r="B171" s="13"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E171" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F171" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="11">
+        <v>38</v>
+      </c>
+      <c r="B172" s="13"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F172" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="13"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F173" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="13"/>
+      <c r="B174" s="13"/>
+      <c r="C174" s="13"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F174" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="13"/>
+      <c r="B175" s="13"/>
+      <c r="C175" s="13"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F175" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="13"/>
+      <c r="B176" s="13"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="12"/>
+      <c r="B177" s="13"/>
+      <c r="C177" s="13"/>
+      <c r="D177" s="12"/>
+      <c r="E177" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F177" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="11">
+        <v>39</v>
+      </c>
+      <c r="B178" s="13"/>
+      <c r="C178" s="13"/>
+      <c r="D178" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E178" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F178" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="13"/>
+      <c r="B179" s="13"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F179" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="12"/>
+      <c r="B180" s="12"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F180" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="A137:A146"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="D137:D146"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="C133:C150"/>
-    <mergeCell ref="B133:B150"/>
+  <mergeCells count="64">
+    <mergeCell ref="D178:D180"/>
+    <mergeCell ref="C133:C180"/>
+    <mergeCell ref="B133:B180"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="A161:A168"/>
+    <mergeCell ref="A169:A170"/>
+    <mergeCell ref="A172:A177"/>
+    <mergeCell ref="A178:A180"/>
+    <mergeCell ref="D151:D155"/>
+    <mergeCell ref="D156:D158"/>
+    <mergeCell ref="D161:D168"/>
+    <mergeCell ref="D169:D170"/>
+    <mergeCell ref="D172:D177"/>
+    <mergeCell ref="D109:D132"/>
+    <mergeCell ref="C54:C132"/>
+    <mergeCell ref="B54:B132"/>
+    <mergeCell ref="A109:A132"/>
+    <mergeCell ref="D96:D108"/>
+    <mergeCell ref="A96:A108"/>
+    <mergeCell ref="D54:D66"/>
+    <mergeCell ref="A54:A66"/>
+    <mergeCell ref="D67:D81"/>
+    <mergeCell ref="D82:D95"/>
+    <mergeCell ref="A67:A81"/>
+    <mergeCell ref="A82:A95"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="C13:C29"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B13:B29"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C2:C12"/>
     <mergeCell ref="D50:D53"/>
     <mergeCell ref="B30:B53"/>
     <mergeCell ref="C30:C53"/>
@@ -3929,36 +4578,12 @@
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="D34:D39"/>
     <mergeCell ref="D41:D43"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="D6:D12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C12"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="C13:C29"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B13:B29"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="D96:D108"/>
-    <mergeCell ref="A96:A108"/>
-    <mergeCell ref="D54:D66"/>
-    <mergeCell ref="A54:A66"/>
-    <mergeCell ref="D67:D81"/>
-    <mergeCell ref="D82:D95"/>
-    <mergeCell ref="A67:A81"/>
-    <mergeCell ref="A82:A95"/>
-    <mergeCell ref="D109:D132"/>
-    <mergeCell ref="C54:C132"/>
-    <mergeCell ref="B54:B132"/>
-    <mergeCell ref="A109:A132"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="A137:A146"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="D137:D146"/>
+    <mergeCell ref="D149:D150"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>